<commit_message>
Added TI part to inventory
</commit_message>
<xml_diff>
--- a/kicad/robot/InventorySent.xlsx
+++ b/kicad/robot/InventorySent.xlsx
@@ -12,7 +12,7 @@
     <sheet name="header" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$6:$F$76</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$6:$F$77</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">Sheet1!$1:$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="224">
   <si>
     <t xml:space="preserve">Inventory</t>
   </si>
@@ -685,6 +685,15 @@
   </si>
   <si>
     <t xml:space="preserve">0.65(L)X0.38(W)X0.36(H) MM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS61253AYFFT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TPS6125xA 3.8-MHz, 5-V / 4-A Boost in 1.2-mm x 1.3-mm WCSP</t>
   </si>
   <si>
     <t xml:space="preserve">Total</t>
@@ -704,6 +713,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -724,22 +734,26 @@
       <sz val="32"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -953,21 +967,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F77"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="bottomLeft" activeCell="F76" activeCellId="0" sqref="F76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="55.85"/>
   </cols>
   <sheetData>
@@ -2464,18 +2478,38 @@
         <v>219</v>
       </c>
     </row>
-    <row r="76" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="16" t="s">
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="18" t="n">
+      <c r="B76" s="11" t="n">
+        <v>25</v>
+      </c>
+      <c r="C76" s="11" t="n">
+        <v>159.37</v>
+      </c>
+      <c r="D76" s="11" t="n">
+        <v>3984</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="16" t="s">
+        <v>223</v>
+      </c>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="18" t="n">
         <f aca="false">SUM(D6:D75)</f>
         <v>38699.7483641476</v>
       </c>
-      <c r="E76" s="19"/>
-      <c r="F76" s="20"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2506,13 +2540,13 @@
       <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="55.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="59.33"/>
   </cols>

</xml_diff>

<commit_message>
Updated Inventory after checking full shipment
</commit_message>
<xml_diff>
--- a/kicad/robot/InventorySent.xlsx
+++ b/kicad/robot/InventorySent.xlsx
@@ -216,7 +216,7 @@
     <t xml:space="preserve">Current Sense Resistors - SMD 5mOhms 1/2W 100PPM/C  0805 AEC-Q200</t>
   </si>
   <si>
-    <t xml:space="preserve">TP1,TP2,TP3,TP4,TP5,T</t>
+    <t xml:space="preserve">TP1,TP2,TP3,TP4,TP5,TP6,TP9,TP10,TP11,TP13,TP14,TP15,TP16,TP17,TP18,TP19,TP20,TP21,TP22,TP23,TP24,TP25,TP26,TP29,TP30,TP31,TP32,TP33,TP34,TP36</t>
   </si>
   <si>
     <t xml:space="preserve">5002</t>
@@ -861,7 +861,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -918,6 +918,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -969,13 +973,13 @@
   </sheetPr>
   <dimension ref="A1:F77"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F76" activeCellId="0" sqref="F76"/>
+      <selection pane="bottomLeft" activeCell="B76" activeCellId="0" sqref="B6:B76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="31.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="9.32"/>
@@ -1290,7 +1294,7 @@
       <c r="A17" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="11" t="n">
+      <c r="B17" s="14" t="n">
         <v>15</v>
       </c>
       <c r="C17" s="13" t="n">
@@ -1311,7 +1315,7 @@
       <c r="A18" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="11" t="n">
+      <c r="B18" s="14" t="n">
         <v>15</v>
       </c>
       <c r="C18" s="13" t="n">
@@ -1332,7 +1336,7 @@
       <c r="A19" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="11" t="n">
+      <c r="B19" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C19" s="13" t="n">
@@ -1353,7 +1357,7 @@
       <c r="A20" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="11" t="n">
+      <c r="B20" s="14" t="n">
         <v>35</v>
       </c>
       <c r="C20" s="13" t="n">
@@ -1374,7 +1378,7 @@
       <c r="A21" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="B21" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C21" s="13" t="n">
@@ -1391,11 +1395,11 @@
         <v>62</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="11" t="s">
+    <row r="22" customFormat="false" ht="15.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="B22" s="14" t="n">
         <v>165</v>
       </c>
       <c r="C22" s="13" t="n">
@@ -1416,7 +1420,7 @@
       <c r="A23" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B23" s="11" t="n">
+      <c r="B23" s="14" t="n">
         <v>25</v>
       </c>
       <c r="C23" s="13" t="n">
@@ -1437,7 +1441,7 @@
       <c r="A24" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B24" s="11" t="n">
+      <c r="B24" s="14" t="n">
         <v>15</v>
       </c>
       <c r="C24" s="13" t="n">
@@ -1458,7 +1462,7 @@
       <c r="A25" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B25" s="11" t="n">
+      <c r="B25" s="14" t="n">
         <v>15</v>
       </c>
       <c r="C25" s="13" t="n">
@@ -1479,7 +1483,7 @@
       <c r="A26" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B26" s="11" t="n">
+      <c r="B26" s="14" t="n">
         <v>35</v>
       </c>
       <c r="C26" s="13" t="n">
@@ -1500,7 +1504,7 @@
       <c r="A27" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="11" t="n">
+      <c r="B27" s="14" t="n">
         <v>50</v>
       </c>
       <c r="C27" s="13" t="n">
@@ -1521,7 +1525,7 @@
       <c r="A28" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="11" t="n">
+      <c r="B28" s="14" t="n">
         <v>15</v>
       </c>
       <c r="C28" s="13" t="n">
@@ -1539,10 +1543,10 @@
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="B29" s="11" t="n">
+      <c r="B29" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C29" s="11" t="n">
@@ -1559,10 +1563,10 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="14" t="s">
+      <c r="A30" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="B30" s="11" t="n">
+      <c r="B30" s="14" t="n">
         <v>56</v>
       </c>
       <c r="C30" s="11" t="n">
@@ -1579,10 +1583,10 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="B31" s="11" t="n">
+      <c r="B31" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C31" s="11" t="n">
@@ -1599,10 +1603,10 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14" t="s">
+      <c r="A32" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="11" t="n">
+      <c r="B32" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C32" s="11" t="n">
@@ -1619,10 +1623,10 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="B33" s="11" t="n">
+      <c r="B33" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C33" s="11" t="n">
@@ -1639,10 +1643,10 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="14" t="s">
+      <c r="A34" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="B34" s="11" t="n">
+      <c r="B34" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C34" s="11" t="n">
@@ -1659,10 +1663,10 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14" t="s">
+      <c r="A35" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="B35" s="11" t="n">
+      <c r="B35" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C35" s="11" t="n">
@@ -1679,10 +1683,10 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="14" t="s">
+      <c r="A36" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="B36" s="11" t="n">
+      <c r="B36" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C36" s="11" t="n">
@@ -1699,10 +1703,10 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14" t="s">
+      <c r="A37" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="B37" s="11" t="n">
+      <c r="B37" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C37" s="11" t="n">
@@ -1719,10 +1723,10 @@
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14" t="s">
+      <c r="A38" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="11" t="n">
+      <c r="B38" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C38" s="11" t="n">
@@ -1739,10 +1743,10 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="14" t="s">
+      <c r="A39" s="15" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="11" t="n">
+      <c r="B39" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C39" s="11" t="n">
@@ -1759,10 +1763,10 @@
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="B40" s="11" t="n">
+      <c r="B40" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C40" s="11" t="n">
@@ -1779,10 +1783,10 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="11" t="n">
+      <c r="B41" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C41" s="11" t="n">
@@ -1799,10 +1803,10 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="B42" s="11" t="n">
+      <c r="B42" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C42" s="11" t="n">
@@ -1819,10 +1823,10 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="11" t="n">
+      <c r="B43" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C43" s="11" t="n">
@@ -1839,10 +1843,10 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B44" s="11" t="n">
+      <c r="B44" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C44" s="11" t="n">
@@ -1859,10 +1863,10 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="15" t="s">
         <v>132</v>
       </c>
-      <c r="B45" s="11" t="n">
+      <c r="B45" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C45" s="11" t="n">
@@ -1879,10 +1883,10 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B46" s="11" t="n">
+      <c r="B46" s="14" t="n">
         <v>100</v>
       </c>
       <c r="C46" s="11" t="n">
@@ -1899,10 +1903,10 @@
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="B47" s="11" t="n">
+      <c r="B47" s="14" t="n">
         <v>100</v>
       </c>
       <c r="C47" s="11" t="n">
@@ -1919,10 +1923,10 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B48" s="11" t="n">
+      <c r="B48" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C48" s="11" t="n">
@@ -1939,10 +1943,10 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="14" t="s">
+      <c r="A49" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="B49" s="11" t="n">
+      <c r="B49" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C49" s="11" t="n">
@@ -1959,10 +1963,10 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="14" t="s">
+      <c r="A50" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="B50" s="11" t="n">
+      <c r="B50" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C50" s="11" t="n">
@@ -1979,10 +1983,10 @@
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="14" t="s">
+      <c r="A51" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="B51" s="11" t="n">
+      <c r="B51" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C51" s="11" t="n">
@@ -1999,10 +2003,10 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="14" t="s">
+      <c r="A52" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B52" s="11" t="n">
+      <c r="B52" s="14" t="n">
         <v>17</v>
       </c>
       <c r="C52" s="11" t="n">
@@ -2019,10 +2023,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="14" t="s">
+      <c r="A53" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="B53" s="11" t="n">
+      <c r="B53" s="14" t="n">
         <v>28</v>
       </c>
       <c r="C53" s="11" t="n">
@@ -2039,10 +2043,10 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="B54" s="11" t="n">
+      <c r="B54" s="14" t="n">
         <v>28</v>
       </c>
       <c r="C54" s="11" t="n">
@@ -2059,10 +2063,10 @@
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="14" t="s">
+      <c r="A55" s="15" t="s">
         <v>162</v>
       </c>
-      <c r="B55" s="11" t="n">
+      <c r="B55" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C55" s="11" t="n">
@@ -2079,10 +2083,10 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="14" t="s">
+      <c r="A56" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="B56" s="11" t="n">
+      <c r="B56" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C56" s="11" t="n">
@@ -2099,10 +2103,10 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="14" t="s">
+      <c r="A57" s="15" t="s">
         <v>168</v>
       </c>
-      <c r="B57" s="11" t="n">
+      <c r="B57" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C57" s="11" t="n">
@@ -2119,10 +2123,10 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="B58" s="11" t="n">
+      <c r="B58" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C58" s="11" t="n">
@@ -2139,10 +2143,10 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="14" t="s">
+      <c r="A59" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="B59" s="11" t="n">
+      <c r="B59" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C59" s="11" t="n">
@@ -2159,10 +2163,10 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="14" t="s">
+      <c r="A60" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="B60" s="11" t="n">
+      <c r="B60" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C60" s="11" t="n">
@@ -2179,10 +2183,10 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="14" t="s">
+      <c r="A61" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="B61" s="11" t="n">
+      <c r="B61" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C61" s="11" t="n">
@@ -2199,10 +2203,10 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="14" t="s">
+      <c r="A62" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="B62" s="11" t="n">
+      <c r="B62" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C62" s="11" t="n">
@@ -2219,10 +2223,10 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="14" t="s">
+      <c r="A63" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="B63" s="11" t="n">
+      <c r="B63" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C63" s="11" t="n">
@@ -2239,10 +2243,10 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="14" t="s">
+      <c r="A64" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="B64" s="11" t="n">
+      <c r="B64" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C64" s="11" t="n">
@@ -2259,10 +2263,10 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="14" t="s">
+      <c r="A65" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="B65" s="11" t="n">
+      <c r="B65" s="14" t="n">
         <v>56</v>
       </c>
       <c r="C65" s="11" t="n">
@@ -2279,10 +2283,10 @@
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="14" t="s">
+      <c r="A66" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="B66" s="11" t="n">
+      <c r="B66" s="14" t="n">
         <v>17</v>
       </c>
       <c r="C66" s="11" t="n">
@@ -2291,7 +2295,7 @@
       <c r="D66" s="11" t="n">
         <v>311</v>
       </c>
-      <c r="E66" s="15" t="n">
+      <c r="E66" s="16" t="n">
         <v>22284030</v>
       </c>
       <c r="F66" s="11" t="s">
@@ -2299,10 +2303,10 @@
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="B67" s="11" t="n">
+      <c r="B67" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C67" s="11" t="n">
@@ -2319,10 +2323,10 @@
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="15" t="s">
         <v>200</v>
       </c>
-      <c r="B68" s="11" t="n">
+      <c r="B68" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C68" s="11" t="n">
@@ -2339,10 +2343,10 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="14" t="s">
+      <c r="A69" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="B69" s="11" t="n">
+      <c r="B69" s="14" t="n">
         <v>39</v>
       </c>
       <c r="C69" s="11" t="n">
@@ -2359,10 +2363,10 @@
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="14" t="s">
+      <c r="A70" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="B70" s="11" t="n">
+      <c r="B70" s="14" t="n">
         <v>11</v>
       </c>
       <c r="C70" s="11" t="n">
@@ -2379,10 +2383,10 @@
       </c>
     </row>
     <row r="71" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="14" t="s">
+      <c r="A71" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="B71" s="11" t="n">
+      <c r="B71" s="14" t="n">
         <v>100</v>
       </c>
       <c r="C71" s="11" t="n">
@@ -2399,10 +2403,10 @@
       </c>
     </row>
     <row r="72" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="14" t="s">
+      <c r="A72" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="B72" s="11" t="n">
+      <c r="B72" s="14" t="n">
         <v>61</v>
       </c>
       <c r="C72" s="11" t="n">
@@ -2419,10 +2423,10 @@
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="14" t="s">
+      <c r="A73" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="B73" s="11" t="n">
+      <c r="B73" s="14" t="n">
         <v>10</v>
       </c>
       <c r="C73" s="11" t="n">
@@ -2439,10 +2443,10 @@
       </c>
     </row>
     <row r="74" customFormat="false" ht="67.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="14" t="s">
+      <c r="A74" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="B74" s="11" t="n">
+      <c r="B74" s="14" t="n">
         <v>226</v>
       </c>
       <c r="C74" s="11" t="n">
@@ -2459,10 +2463,10 @@
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="14" t="s">
+      <c r="A75" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="B75" s="11" t="n">
+      <c r="B75" s="14" t="n">
         <v>6</v>
       </c>
       <c r="C75" s="11" t="n">
@@ -2479,10 +2483,10 @@
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="14" t="s">
+      <c r="A76" s="15" t="s">
         <v>220</v>
       </c>
-      <c r="B76" s="11" t="n">
+      <c r="B76" s="14" t="n">
         <v>25</v>
       </c>
       <c r="C76" s="11" t="n">
@@ -2499,17 +2503,17 @@
       </c>
     </row>
     <row r="77" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="16" t="s">
+      <c r="A77" s="17" t="s">
         <v>223</v>
       </c>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="18" t="n">
+      <c r="B77" s="18"/>
+      <c r="C77" s="18"/>
+      <c r="D77" s="19" t="n">
         <f aca="false">SUM(D6:D75)</f>
         <v>38699.7483641476</v>
       </c>
-      <c r="E77" s="19"/>
-      <c r="F77" s="20"/>
+      <c r="E77" s="20"/>
+      <c r="F77" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2536,14 +2540,14 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="1" sqref="B6:B76 A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="32.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="7.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.06"/>
@@ -2602,22 +2606,22 @@
       <c r="F4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="21" t="s">
+      <c r="F5" s="22" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>